<commit_message>
Migraciones relacion de etiquetas y estudios
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/seed/03_CAT_ETIQUETAS.xlsx
+++ b/Service.Catalog/wwwroot/seed/03_CAT_ETIQUETAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-71\source\repos\LaboratorioRamos\API\Service.Catalog\wwwroot\seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03B020B-23FB-4BED-AAEB-65A7DE3B602F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B104D58-F17D-4C0D-B05F-53DEC4ACA923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETIQUETAS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="259">
   <si>
     <t>TTL</t>
   </si>
@@ -796,6 +796,18 @@
   </si>
   <si>
     <t>#F0D560</t>
+  </si>
+  <si>
+    <t>ClaveInicial</t>
+  </si>
+  <si>
+    <t>23 (año)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>23(año)</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1297,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
       <right style="thin">
         <color theme="4"/>
       </right>
@@ -1296,7 +1310,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
       <right style="thin">
         <color theme="4"/>
       </right>
@@ -1353,7 +1369,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1361,9 +1377,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1719,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,9 +1749,10 @@
     <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>241</v>
       </c>
@@ -1747,11 +1765,14 @@
       <c r="D1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1764,11 +1785,14 @@
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1781,9 +1805,12 @@
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1796,9 +1823,12 @@
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="4"/>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1811,9 +1841,12 @@
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+      <c r="F5" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1826,9 +1859,12 @@
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="4"/>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1841,9 +1877,12 @@
       <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="4"/>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1856,11 +1895,14 @@
       <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1873,9 +1915,12 @@
       <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+      <c r="F9" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1888,9 +1933,12 @@
       <c r="D10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1903,9 +1951,12 @@
       <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1918,11 +1969,14 @@
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1935,9 +1989,12 @@
       <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="F13" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1950,9 +2007,12 @@
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1965,9 +2025,12 @@
       <c r="D15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+      <c r="F15" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1980,9 +2043,12 @@
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+      <c r="F16" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1995,11 +2061,14 @@
       <c r="D17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2012,11 +2081,14 @@
       <c r="D18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2029,9 +2101,12 @@
       <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+      <c r="F19" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2044,9 +2119,12 @@
       <c r="D20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
+      <c r="F20" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2059,9 +2137,12 @@
       <c r="D21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="F21" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2074,9 +2155,12 @@
       <c r="D22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="F22" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2089,9 +2173,12 @@
       <c r="D23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+      <c r="F23" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2104,9 +2191,12 @@
       <c r="D24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+      <c r="F24" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2119,9 +2209,12 @@
       <c r="D25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
+      <c r="F25" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2134,11 +2227,14 @@
       <c r="D26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2151,11 +2247,14 @@
       <c r="D27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2168,9 +2267,12 @@
       <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+      <c r="F28" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2183,9 +2285,12 @@
       <c r="D29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="4"/>
+      <c r="F29" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2198,11 +2303,14 @@
       <c r="D30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2215,11 +2323,14 @@
       <c r="D31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2232,11 +2343,14 @@
       <c r="D32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2249,9 +2363,12 @@
       <c r="D33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="4"/>
+      <c r="F33" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2264,11 +2381,14 @@
       <c r="D34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2281,9 +2401,12 @@
       <c r="D35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="4"/>
+      <c r="F35" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2296,9 +2419,12 @@
       <c r="D36" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="4"/>
+      <c r="F36" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2311,9 +2437,12 @@
       <c r="D37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
+      <c r="F37" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2326,9 +2455,12 @@
       <c r="D38" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
+      <c r="F38" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2341,9 +2473,12 @@
       <c r="D39" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="4"/>
+      <c r="F39" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2356,9 +2491,12 @@
       <c r="D40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="4"/>
+      <c r="F40" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2371,11 +2509,14 @@
       <c r="D41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2388,9 +2529,12 @@
       <c r="D42" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="4"/>
+      <c r="F42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2403,9 +2547,12 @@
       <c r="D43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="4"/>
+      <c r="F43" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2418,9 +2565,12 @@
       <c r="D44" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="4"/>
+      <c r="F44" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2433,11 +2583,14 @@
       <c r="D45" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2450,11 +2603,14 @@
       <c r="D46" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2467,11 +2623,14 @@
       <c r="D47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2484,11 +2643,14 @@
       <c r="D48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2501,11 +2663,14 @@
       <c r="D49" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2518,11 +2683,14 @@
       <c r="D50" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2535,11 +2703,14 @@
       <c r="D51" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2552,11 +2723,14 @@
       <c r="D52" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2569,11 +2743,14 @@
       <c r="D53" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -2586,11 +2763,14 @@
       <c r="D54" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -2603,11 +2783,14 @@
       <c r="D55" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -2620,9 +2803,12 @@
       <c r="D56" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="4"/>
+      <c r="F56" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -2635,9 +2821,12 @@
       <c r="D57" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="4"/>
+      <c r="F57" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -2650,9 +2839,12 @@
       <c r="D58" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="4"/>
+      <c r="F58" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -2665,11 +2857,14 @@
       <c r="D59" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -2682,9 +2877,12 @@
       <c r="D60" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E60" s="8"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="4"/>
+      <c r="F60" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -2697,9 +2895,12 @@
       <c r="D61" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="4"/>
+      <c r="F61" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -2712,11 +2913,14 @@
       <c r="D62" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -2729,11 +2933,14 @@
       <c r="D63" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -2746,11 +2953,14 @@
       <c r="D64" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E64" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -2763,11 +2973,14 @@
       <c r="D65" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E65" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -2780,11 +2993,14 @@
       <c r="D66" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E66" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -2797,9 +3013,12 @@
       <c r="D67" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="4"/>
+      <c r="F67" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -2812,11 +3031,14 @@
       <c r="D68" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E68" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -2829,11 +3051,14 @@
       <c r="D69" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E69" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -2846,9 +3071,12 @@
       <c r="D70" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E70" s="8"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="4"/>
+      <c r="F70" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -2861,9 +3089,12 @@
       <c r="D71" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E71" s="8"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="4"/>
+      <c r="F71" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -2876,9 +3107,12 @@
       <c r="D72" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="4"/>
+      <c r="F72" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -2891,11 +3125,14 @@
       <c r="D73" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -2908,11 +3145,14 @@
       <c r="D74" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E74" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -2925,9 +3165,12 @@
       <c r="D75" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E75" s="8"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="4"/>
+      <c r="F75" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -2940,11 +3183,14 @@
       <c r="D76" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E76" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -2957,9 +3203,12 @@
       <c r="D77" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E77" s="8"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="4"/>
+      <c r="F77" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -2972,9 +3221,12 @@
       <c r="D78" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E78" s="8"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="4"/>
+      <c r="F78" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -2987,9 +3239,12 @@
       <c r="D79" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="4"/>
+      <c r="F79" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3002,9 +3257,12 @@
       <c r="D80" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E80" s="8"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="4"/>
+      <c r="F80" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -3017,9 +3275,12 @@
       <c r="D81" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E81" s="8"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="4"/>
+      <c r="F81" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -3032,9 +3293,12 @@
       <c r="D82" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E82" s="8"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="4"/>
+      <c r="F82" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -3047,9 +3311,12 @@
       <c r="D83" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E83" s="8"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="4"/>
+      <c r="F83" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -3062,9 +3329,12 @@
       <c r="D84" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E84" s="8"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="4"/>
+      <c r="F84" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -3077,9 +3347,12 @@
       <c r="D85" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E85" s="8"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="4"/>
+      <c r="F85" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -3092,9 +3365,12 @@
       <c r="D86" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E86" s="8"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="4"/>
+      <c r="F86" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -3107,11 +3383,14 @@
       <c r="D87" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -3124,9 +3403,12 @@
       <c r="D88" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E88" s="8"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="4"/>
+      <c r="F88" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -3139,9 +3421,12 @@
       <c r="D89" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E89" s="8"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="4"/>
+      <c r="F89" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -3154,11 +3439,14 @@
       <c r="D90" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="E90" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -3171,9 +3459,12 @@
       <c r="D91" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E91" s="8"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="4"/>
+      <c r="F91" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -3186,9 +3477,12 @@
       <c r="D92" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E92" s="8"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="4"/>
+      <c r="F92" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -3201,9 +3495,12 @@
       <c r="D93" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E93" s="8"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="4"/>
+      <c r="F93" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -3216,9 +3513,12 @@
       <c r="D94" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="E94" s="8"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="4"/>
+      <c r="F94" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -3231,9 +3531,12 @@
       <c r="D95" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E95" s="8"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="4"/>
+      <c r="F95" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -3246,9 +3549,12 @@
       <c r="D96" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E96" s="8"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="4"/>
+      <c r="F96" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -3261,9 +3567,12 @@
       <c r="D97" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E97" s="8"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="4"/>
+      <c r="F97" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -3276,9 +3585,12 @@
       <c r="D98" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E98" s="8"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="4"/>
+      <c r="F98" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -3291,11 +3603,14 @@
       <c r="D99" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E99" s="8" t="s">
+      <c r="E99" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -3308,11 +3623,14 @@
       <c r="D100" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="E100" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -3325,11 +3643,14 @@
       <c r="D101" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="E101" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -3342,11 +3663,14 @@
       <c r="D102" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E102" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -3359,11 +3683,14 @@
       <c r="D103" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E103" s="8" t="s">
+      <c r="E103" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -3376,11 +3703,14 @@
       <c r="D104" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="E104" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -3393,11 +3723,14 @@
       <c r="D105" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E105" s="8" t="s">
+      <c r="E105" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -3410,11 +3743,14 @@
       <c r="D106" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E106" s="8" t="s">
+      <c r="E106" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -3427,11 +3763,14 @@
       <c r="D107" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E107" s="8" t="s">
+      <c r="E107" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -3444,9 +3783,12 @@
       <c r="D108" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E108" s="8"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="4"/>
+      <c r="F108" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -3459,9 +3801,12 @@
       <c r="D109" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E109" s="8"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="4"/>
+      <c r="F109" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -3474,11 +3819,14 @@
       <c r="D110" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E110" s="8" t="s">
+      <c r="E110" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -3491,9 +3839,12 @@
       <c r="D111" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E111" s="8"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="4"/>
+      <c r="F111" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -3506,9 +3857,12 @@
       <c r="D112" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E112" s="8"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="4"/>
+      <c r="F112" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -3521,9 +3875,12 @@
       <c r="D113" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E113" s="8"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="4"/>
+      <c r="F113" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -3536,9 +3893,12 @@
       <c r="D114" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E114" s="8"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="4"/>
+      <c r="F114" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -3551,9 +3911,12 @@
       <c r="D115" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E115" s="8"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="4"/>
+      <c r="F115" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -3566,9 +3929,12 @@
       <c r="D116" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="E116" s="8"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="4"/>
+      <c r="F116" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -3581,9 +3947,12 @@
       <c r="D117" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="E117" s="8"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="4"/>
+      <c r="F117" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -3596,9 +3965,12 @@
       <c r="D118" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="E118" s="8"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="4"/>
+      <c r="F118" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -3611,9 +3983,12 @@
       <c r="D119" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="E119" s="8"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="4"/>
+      <c r="F119" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -3626,11 +4001,14 @@
       <c r="D120" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="E120" s="8" t="s">
+      <c r="E120" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -3643,11 +4021,14 @@
       <c r="D121" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="E121" s="8" t="s">
+      <c r="E121" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -3660,9 +4041,12 @@
       <c r="D122" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E122" s="8"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="4"/>
+      <c r="F122" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -3675,9 +4059,12 @@
       <c r="D123" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="E123" s="8"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="4"/>
+      <c r="F123" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -3690,9 +4077,12 @@
       <c r="D124" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E124" s="8"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="4"/>
+      <c r="F124" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -3705,11 +4095,14 @@
       <c r="D125" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E125" s="8" t="s">
+      <c r="E125" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -3722,11 +4115,14 @@
       <c r="D126" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E126" s="8" t="s">
+      <c r="E126" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -3739,9 +4135,12 @@
       <c r="D127" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E127" s="8"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="4"/>
+      <c r="F127" s="8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -3754,11 +4153,14 @@
       <c r="D128" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E128" s="8" t="s">
+      <c r="E128" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128" s="8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -3771,9 +4173,12 @@
       <c r="D129" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="E129" s="8"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="4"/>
+      <c r="F129" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -3786,9 +4191,12 @@
       <c r="D130" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E130" s="8"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="4"/>
+      <c r="F130" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -3801,11 +4209,14 @@
       <c r="D131" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="E131" s="8" t="s">
+      <c r="E131" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -3818,9 +4229,12 @@
       <c r="D132" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="E132" s="8"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="4"/>
+      <c r="F132" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -3833,7 +4247,10 @@
       <c r="D133" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="E133" s="9"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="9">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Feat] Cobro y Noificacion de respuesta NetPay
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/seed/03_CAT_ETIQUETAS.xlsx
+++ b/Service.Catalog/wwwroot/seed/03_CAT_ETIQUETAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-71\source\repos\LaboratorioRamos\API\Service.Catalog\wwwroot\seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03B020B-23FB-4BED-AAEB-65A7DE3B602F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B104D58-F17D-4C0D-B05F-53DEC4ACA923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ETIQUETAS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="259">
   <si>
     <t>TTL</t>
   </si>
@@ -796,6 +796,18 @@
   </si>
   <si>
     <t>#F0D560</t>
+  </si>
+  <si>
+    <t>ClaveInicial</t>
+  </si>
+  <si>
+    <t>23 (año)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>23(año)</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1297,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
       <right style="thin">
         <color theme="4"/>
       </right>
@@ -1296,7 +1310,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
       <right style="thin">
         <color theme="4"/>
       </right>
@@ -1353,7 +1369,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1361,9 +1377,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1719,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,9 +1749,10 @@
     <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>241</v>
       </c>
@@ -1747,11 +1765,14 @@
       <c r="D1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1764,11 +1785,14 @@
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1781,9 +1805,12 @@
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1796,9 +1823,12 @@
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="4"/>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1811,9 +1841,12 @@
       <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+      <c r="F5" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1826,9 +1859,12 @@
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="4"/>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1841,9 +1877,12 @@
       <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="4"/>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1856,11 +1895,14 @@
       <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1873,9 +1915,12 @@
       <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+      <c r="F9" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1888,9 +1933,12 @@
       <c r="D10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1903,9 +1951,12 @@
       <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1918,11 +1969,14 @@
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1935,9 +1989,12 @@
       <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="F13" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1950,9 +2007,12 @@
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1965,9 +2025,12 @@
       <c r="D15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+      <c r="F15" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1980,9 +2043,12 @@
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+      <c r="F16" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1995,11 +2061,14 @@
       <c r="D17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2012,11 +2081,14 @@
       <c r="D18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2029,9 +2101,12 @@
       <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+      <c r="F19" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2044,9 +2119,12 @@
       <c r="D20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
+      <c r="F20" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2059,9 +2137,12 @@
       <c r="D21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="F21" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2074,9 +2155,12 @@
       <c r="D22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="F22" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2089,9 +2173,12 @@
       <c r="D23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+      <c r="F23" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2104,9 +2191,12 @@
       <c r="D24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+      <c r="F24" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2119,9 +2209,12 @@
       <c r="D25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
+      <c r="F25" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2134,11 +2227,14 @@
       <c r="D26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2151,11 +2247,14 @@
       <c r="D27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2168,9 +2267,12 @@
       <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+      <c r="F28" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2183,9 +2285,12 @@
       <c r="D29" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="4"/>
+      <c r="F29" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2198,11 +2303,14 @@
       <c r="D30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2215,11 +2323,14 @@
       <c r="D31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2232,11 +2343,14 @@
       <c r="D32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2249,9 +2363,12 @@
       <c r="D33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="4"/>
+      <c r="F33" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2264,11 +2381,14 @@
       <c r="D34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2281,9 +2401,12 @@
       <c r="D35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="4"/>
+      <c r="F35" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2296,9 +2419,12 @@
       <c r="D36" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="4"/>
+      <c r="F36" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2311,9 +2437,12 @@
       <c r="D37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
+      <c r="F37" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2326,9 +2455,12 @@
       <c r="D38" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
+      <c r="F38" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2341,9 +2473,12 @@
       <c r="D39" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="4"/>
+      <c r="F39" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2356,9 +2491,12 @@
       <c r="D40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="4"/>
+      <c r="F40" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2371,11 +2509,14 @@
       <c r="D41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2388,9 +2529,12 @@
       <c r="D42" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="4"/>
+      <c r="F42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2403,9 +2547,12 @@
       <c r="D43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="4"/>
+      <c r="F43" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2418,9 +2565,12 @@
       <c r="D44" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="4"/>
+      <c r="F44" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2433,11 +2583,14 @@
       <c r="D45" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2450,11 +2603,14 @@
       <c r="D46" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2467,11 +2623,14 @@
       <c r="D47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2484,11 +2643,14 @@
       <c r="D48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2501,11 +2663,14 @@
       <c r="D49" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2518,11 +2683,14 @@
       <c r="D50" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2535,11 +2703,14 @@
       <c r="D51" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2552,11 +2723,14 @@
       <c r="D52" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2569,11 +2743,14 @@
       <c r="D53" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -2586,11 +2763,14 @@
       <c r="D54" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -2603,11 +2783,14 @@
       <c r="D55" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -2620,9 +2803,12 @@
       <c r="D56" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="4"/>
+      <c r="F56" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -2635,9 +2821,12 @@
       <c r="D57" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="4"/>
+      <c r="F57" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -2650,9 +2839,12 @@
       <c r="D58" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="4"/>
+      <c r="F58" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -2665,11 +2857,14 @@
       <c r="D59" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -2682,9 +2877,12 @@
       <c r="D60" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E60" s="8"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="4"/>
+      <c r="F60" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -2697,9 +2895,12 @@
       <c r="D61" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="4"/>
+      <c r="F61" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -2712,11 +2913,14 @@
       <c r="D62" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -2729,11 +2933,14 @@
       <c r="D63" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -2746,11 +2953,14 @@
       <c r="D64" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E64" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -2763,11 +2973,14 @@
       <c r="D65" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E65" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -2780,11 +2993,14 @@
       <c r="D66" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E66" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -2797,9 +3013,12 @@
       <c r="D67" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="4"/>
+      <c r="F67" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -2812,11 +3031,14 @@
       <c r="D68" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E68" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -2829,11 +3051,14 @@
       <c r="D69" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E69" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -2846,9 +3071,12 @@
       <c r="D70" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E70" s="8"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="4"/>
+      <c r="F70" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -2861,9 +3089,12 @@
       <c r="D71" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E71" s="8"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="4"/>
+      <c r="F71" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -2876,9 +3107,12 @@
       <c r="D72" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="4"/>
+      <c r="F72" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -2891,11 +3125,14 @@
       <c r="D73" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -2908,11 +3145,14 @@
       <c r="D74" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E74" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -2925,9 +3165,12 @@
       <c r="D75" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E75" s="8"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="4"/>
+      <c r="F75" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -2940,11 +3183,14 @@
       <c r="D76" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E76" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -2957,9 +3203,12 @@
       <c r="D77" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E77" s="8"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="4"/>
+      <c r="F77" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -2972,9 +3221,12 @@
       <c r="D78" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E78" s="8"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="4"/>
+      <c r="F78" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -2987,9 +3239,12 @@
       <c r="D79" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="4"/>
+      <c r="F79" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3002,9 +3257,12 @@
       <c r="D80" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E80" s="8"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="4"/>
+      <c r="F80" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -3017,9 +3275,12 @@
       <c r="D81" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E81" s="8"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="4"/>
+      <c r="F81" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -3032,9 +3293,12 @@
       <c r="D82" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E82" s="8"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="4"/>
+      <c r="F82" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -3047,9 +3311,12 @@
       <c r="D83" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E83" s="8"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="4"/>
+      <c r="F83" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -3062,9 +3329,12 @@
       <c r="D84" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E84" s="8"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="4"/>
+      <c r="F84" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -3077,9 +3347,12 @@
       <c r="D85" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E85" s="8"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="4"/>
+      <c r="F85" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -3092,9 +3365,12 @@
       <c r="D86" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E86" s="8"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="4"/>
+      <c r="F86" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -3107,11 +3383,14 @@
       <c r="D87" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -3124,9 +3403,12 @@
       <c r="D88" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E88" s="8"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="4"/>
+      <c r="F88" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -3139,9 +3421,12 @@
       <c r="D89" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E89" s="8"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="4"/>
+      <c r="F89" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -3154,11 +3439,14 @@
       <c r="D90" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="E90" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -3171,9 +3459,12 @@
       <c r="D91" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E91" s="8"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="4"/>
+      <c r="F91" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -3186,9 +3477,12 @@
       <c r="D92" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E92" s="8"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="4"/>
+      <c r="F92" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -3201,9 +3495,12 @@
       <c r="D93" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E93" s="8"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="4"/>
+      <c r="F93" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -3216,9 +3513,12 @@
       <c r="D94" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="E94" s="8"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="4"/>
+      <c r="F94" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -3231,9 +3531,12 @@
       <c r="D95" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E95" s="8"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="4"/>
+      <c r="F95" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -3246,9 +3549,12 @@
       <c r="D96" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E96" s="8"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="4"/>
+      <c r="F96" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -3261,9 +3567,12 @@
       <c r="D97" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E97" s="8"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="4"/>
+      <c r="F97" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -3276,9 +3585,12 @@
       <c r="D98" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E98" s="8"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="4"/>
+      <c r="F98" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -3291,11 +3603,14 @@
       <c r="D99" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E99" s="8" t="s">
+      <c r="E99" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -3308,11 +3623,14 @@
       <c r="D100" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="E100" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -3325,11 +3643,14 @@
       <c r="D101" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="E101" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -3342,11 +3663,14 @@
       <c r="D102" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E102" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -3359,11 +3683,14 @@
       <c r="D103" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E103" s="8" t="s">
+      <c r="E103" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -3376,11 +3703,14 @@
       <c r="D104" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="E104" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -3393,11 +3723,14 @@
       <c r="D105" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E105" s="8" t="s">
+      <c r="E105" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -3410,11 +3743,14 @@
       <c r="D106" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E106" s="8" t="s">
+      <c r="E106" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -3427,11 +3763,14 @@
       <c r="D107" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E107" s="8" t="s">
+      <c r="E107" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -3444,9 +3783,12 @@
       <c r="D108" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E108" s="8"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="4"/>
+      <c r="F108" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -3459,9 +3801,12 @@
       <c r="D109" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E109" s="8"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="4"/>
+      <c r="F109" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -3474,11 +3819,14 @@
       <c r="D110" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E110" s="8" t="s">
+      <c r="E110" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -3491,9 +3839,12 @@
       <c r="D111" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E111" s="8"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="4"/>
+      <c r="F111" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -3506,9 +3857,12 @@
       <c r="D112" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E112" s="8"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="4"/>
+      <c r="F112" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -3521,9 +3875,12 @@
       <c r="D113" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E113" s="8"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="4"/>
+      <c r="F113" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -3536,9 +3893,12 @@
       <c r="D114" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E114" s="8"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="4"/>
+      <c r="F114" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -3551,9 +3911,12 @@
       <c r="D115" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E115" s="8"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="4"/>
+      <c r="F115" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -3566,9 +3929,12 @@
       <c r="D116" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="E116" s="8"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="4"/>
+      <c r="F116" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -3581,9 +3947,12 @@
       <c r="D117" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="E117" s="8"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="4"/>
+      <c r="F117" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -3596,9 +3965,12 @@
       <c r="D118" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="E118" s="8"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="4"/>
+      <c r="F118" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -3611,9 +3983,12 @@
       <c r="D119" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="E119" s="8"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="4"/>
+      <c r="F119" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -3626,11 +4001,14 @@
       <c r="D120" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="E120" s="8" t="s">
+      <c r="E120" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -3643,11 +4021,14 @@
       <c r="D121" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="E121" s="8" t="s">
+      <c r="E121" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -3660,9 +4041,12 @@
       <c r="D122" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E122" s="8"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="4"/>
+      <c r="F122" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -3675,9 +4059,12 @@
       <c r="D123" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="E123" s="8"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="4"/>
+      <c r="F123" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -3690,9 +4077,12 @@
       <c r="D124" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E124" s="8"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="4"/>
+      <c r="F124" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -3705,11 +4095,14 @@
       <c r="D125" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E125" s="8" t="s">
+      <c r="E125" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -3722,11 +4115,14 @@
       <c r="D126" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E126" s="8" t="s">
+      <c r="E126" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -3739,9 +4135,12 @@
       <c r="D127" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E127" s="8"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="4"/>
+      <c r="F127" s="8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -3754,11 +4153,14 @@
       <c r="D128" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E128" s="8" t="s">
+      <c r="E128" s="4" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128" s="8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -3771,9 +4173,12 @@
       <c r="D129" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="E129" s="8"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="4"/>
+      <c r="F129" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -3786,9 +4191,12 @@
       <c r="D130" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E130" s="8"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="4"/>
+      <c r="F130" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -3801,11 +4209,14 @@
       <c r="D131" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="E131" s="8" t="s">
+      <c r="E131" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -3818,9 +4229,12 @@
       <c r="D132" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="E132" s="8"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="4"/>
+      <c r="F132" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -3833,7 +4247,10 @@
       <c r="D133" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="E133" s="9"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="9">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>